<commit_message>
Add duplicated Id check Add invalid type check Add unparseable data check Add bool support(0,1,T,F,true,false)
</commit_message>
<xml_diff>
--- a/excels/SimpleTypes.xlsx
+++ b/excels/SimpleTypes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="460" windowWidth="32520" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="9200" yWindow="1340" windowWidth="30660" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="104">
   <si>
     <t>KEY</t>
   </si>
@@ -307,6 +307,39 @@
   </si>
   <si>
     <t>{item0_1=fse|item0_2=fsd}|{item1_1=qwe|item1_2=qse}</t>
+  </si>
+  <si>
+    <t>1003</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>list&lt;string&gt;:3</t>
+  </si>
+  <si>
+    <t>BOOLS</t>
+  </si>
+  <si>
+    <t>BoolTest</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  8.9</t>
   </si>
 </sst>
 </file>
@@ -765,13 +798,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ5"/>
+  <dimension ref="A1:AS6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,44 +813,46 @@
     <col min="2" max="2" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="20" style="1" customWidth="1"/>
-    <col min="18" max="18" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.6640625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="20.83203125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="46.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.83203125" style="1" customWidth="1"/>
-    <col min="35" max="35" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="24.83203125" style="1" customWidth="1"/>
-    <col min="39" max="39" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.83203125" style="1"/>
-    <col min="43" max="43" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="8.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="52.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="20" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="20.83203125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="33" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="80.1640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.83203125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="24.83203125" style="1" customWidth="1"/>
+    <col min="41" max="41" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.83203125" style="1"/>
+    <col min="45" max="45" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="26.1640625" style="1" customWidth="1"/>
+    <col min="47" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -830,75 +865,79 @@
       <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13"/>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="13"/>
+      <c r="J1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="14"/>
       <c r="L1" s="14"/>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
       <c r="Q1" s="15"/>
       <c r="R1" s="15"/>
       <c r="S1" s="15"/>
       <c r="T1" s="15"/>
-      <c r="U1" s="16" t="s">
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="12" t="s">
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" s="17" t="s">
+      <c r="AA1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
       <c r="AB1" s="17"/>
       <c r="AC1" s="17"/>
       <c r="AD1" s="17"/>
       <c r="AE1" s="17"/>
-      <c r="AF1" s="18" t="s">
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="12" t="s">
+      <c r="AI1" s="18"/>
+      <c r="AJ1" s="18"/>
+      <c r="AK1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="AJ1" s="19" t="s">
+      <c r="AL1" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="20" t="s">
+      <c r="AM1" s="19"/>
+      <c r="AN1" s="19"/>
+      <c r="AO1" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="AN1" s="21" t="s">
+      <c r="AP1" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="AO1" s="21"/>
-      <c r="AP1" s="21"/>
-      <c r="AQ1" s="20" t="s">
+      <c r="AQ1" s="21"/>
+      <c r="AR1" s="21"/>
+      <c r="AS1" s="20" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
@@ -911,105 +950,109 @@
       <c r="D2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="14"/>
       <c r="L2" s="14"/>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="P2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="Q2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="R2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="S2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="T2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="U2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="V2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="W2" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="X2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="Y2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="Z2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" s="17" t="s">
+      <c r="AA2" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="17" t="s">
+      <c r="AB2" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="17"/>
-      <c r="AC2" s="17" t="s">
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17"/>
+      <c r="AE2" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="AD2" s="17"/>
-      <c r="AE2" s="17"/>
-      <c r="AF2" s="18" t="s">
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="17"/>
+      <c r="AH2" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="AG2" s="18"/>
-      <c r="AH2" s="18"/>
-      <c r="AI2" s="12" t="s">
+      <c r="AI2" s="18"/>
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AJ2" s="19" t="s">
+      <c r="AL2" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="AK2" s="19" t="s">
+      <c r="AM2" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="AL2" s="19" t="s">
+      <c r="AN2" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="AM2" s="20" t="s">
+      <c r="AO2" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="AN2" s="21" t="s">
+      <c r="AP2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="AO2" s="21"/>
-      <c r="AP2" s="21"/>
-      <c r="AQ2" s="20" t="s">
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21"/>
+      <c r="AS2" s="20" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>19</v>
       </c>
@@ -1022,182 +1065,192 @@
       <c r="D3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="13"/>
+      <c r="J3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="14"/>
+      <c r="K3" s="14" t="s">
+        <v>95</v>
+      </c>
       <c r="L3" s="14"/>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="P3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
       <c r="S3" s="15"/>
       <c r="T3" s="15"/>
-      <c r="U3" s="16" t="s">
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
-      <c r="X3" s="12" t="s">
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="Y3" s="17" t="s">
+      <c r="AA3" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="17"/>
       <c r="AB3" s="17"/>
       <c r="AC3" s="17"/>
       <c r="AD3" s="17"/>
       <c r="AE3" s="17"/>
-      <c r="AF3" s="18" t="s">
+      <c r="AF3" s="17"/>
+      <c r="AG3" s="17"/>
+      <c r="AH3" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="AG3" s="18"/>
-      <c r="AH3" s="18"/>
-      <c r="AI3" s="12" t="s">
+      <c r="AI3" s="18"/>
+      <c r="AJ3" s="18"/>
+      <c r="AK3" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="AJ3" s="19" t="s">
+      <c r="AL3" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="AK3" s="19"/>
-      <c r="AL3" s="19"/>
-      <c r="AM3" s="20" t="s">
+      <c r="AM3" s="19"/>
+      <c r="AN3" s="19"/>
+      <c r="AO3" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="AN3" s="21" t="s">
+      <c r="AP3" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="AO3" s="21"/>
-      <c r="AP3" s="21"/>
-      <c r="AQ3" s="20" t="s">
+      <c r="AQ3" s="21"/>
+      <c r="AR3" s="21"/>
+      <c r="AS3" s="20" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:43" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="20">
         <v>1001</v>
       </c>
-      <c r="B4" s="20">
-        <v>1</v>
+      <c r="B4" s="20" t="s">
+        <v>102</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="20">
-        <v>8.9</v>
-      </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20">
+      <c r="D4" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20">
         <v>3.33</v>
       </c>
-      <c r="G4" s="20">
+      <c r="H4" s="20">
         <v>4.4400000000000004</v>
       </c>
-      <c r="H4" s="20">
+      <c r="I4" s="20">
         <v>5.55</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="J4" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="20"/>
+      <c r="L4" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="M4" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="N4" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20" t="s">
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="Q4" s="20" t="s">
+      <c r="S4" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20" t="s">
+      <c r="T4" s="20"/>
+      <c r="U4" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="T4" s="20" t="s">
+      <c r="V4" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="U4" s="20"/>
-      <c r="V4" s="20" t="s">
+      <c r="W4" s="20"/>
+      <c r="X4" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="W4" s="20" t="s">
+      <c r="Y4" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="X4" s="20" t="s">
+      <c r="Z4" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="20" t="s">
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="20"/>
+      <c r="AC4" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AB4" s="20" t="s">
+      <c r="AD4" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="20" t="s">
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="AE4" s="20" t="s">
+      <c r="AG4" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="AF4" s="20"/>
-      <c r="AG4" s="20" t="s">
+      <c r="AH4" s="20"/>
+      <c r="AI4" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="AH4" s="20" t="s">
+      <c r="AJ4" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AI4" s="20" t="s">
+      <c r="AK4" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="AJ4" s="20"/>
-      <c r="AK4" s="20" t="s">
+      <c r="AL4" s="20"/>
+      <c r="AM4" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="AL4" s="20" t="s">
+      <c r="AN4" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="AM4" s="20" t="s">
+      <c r="AO4" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="AN4" s="20"/>
-      <c r="AO4" s="20" t="s">
+      <c r="AP4" s="20"/>
+      <c r="AQ4" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="AP4" s="20" t="s">
+      <c r="AR4" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="AQ4" s="20" t="s">
+      <c r="AS4" s="20" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="20">
         <v>1002</v>
       </c>
@@ -1210,97 +1263,216 @@
       <c r="D5" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20" t="s">
+      <c r="E5" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="H5" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="I5" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="J5" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="20"/>
+      <c r="L5" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="M5" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="20" t="s">
+      <c r="N5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20" t="s">
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="Q5" s="20" t="s">
+      <c r="S5" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20" t="s">
+      <c r="T5" s="20"/>
+      <c r="U5" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="T5" s="20" t="s">
+      <c r="V5" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="U5" s="20"/>
-      <c r="V5" s="20" t="s">
+      <c r="W5" s="20"/>
+      <c r="X5" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="W5" s="20" t="s">
+      <c r="Y5" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="X5" s="20" t="s">
+      <c r="Z5" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="20"/>
-      <c r="AA5" s="20" t="s">
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AB5" s="20" t="s">
+      <c r="AD5" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AC5" s="20"/>
-      <c r="AD5" s="20" t="s">
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="AE5" s="20" t="s">
+      <c r="AG5" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="AF5" s="20"/>
-      <c r="AG5" s="20" t="s">
+      <c r="AH5" s="20"/>
+      <c r="AI5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="AH5" s="20" t="s">
+      <c r="AJ5" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AI5" s="20" t="s">
+      <c r="AK5" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="AJ5" s="20"/>
-      <c r="AK5" s="20" t="s">
+      <c r="AL5" s="20"/>
+      <c r="AM5" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="AL5" s="20" t="s">
+      <c r="AN5" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="AM5" s="20" t="s">
+      <c r="AO5" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="AN5" s="20"/>
-      <c r="AO5" s="20" t="s">
+      <c r="AP5" s="20"/>
+      <c r="AQ5" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="AP5" s="20" t="s">
+      <c r="AR5" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="AQ5" s="20" t="s">
+      <c r="AS5" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="20">
+        <v>2</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="S6" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="V6" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="W6" s="20"/>
+      <c r="X6" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y6" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD6" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG6" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH6" s="20"/>
+      <c r="AI6" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ6" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK6" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL6" s="20"/>
+      <c r="AM6" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="AN6" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AO6" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP6" s="20"/>
+      <c r="AQ6" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR6" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS6" s="20" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>